<commit_message>
removed pass fail coloumn
</commit_message>
<xml_diff>
--- a/QATCAndQATP/QATC_for_Gapstars_Assignment.xlsx
+++ b/QATCAndQATP/QATC_for_Gapstars_Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\it17145930\GapstarWorkspace\QATCAndQATP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075F34CE-4E18-4C28-A663-37A2B7066A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681E4913-199D-4065-A2A2-D422815FB5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Featured Description</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Pass/Fail Staus</t>
   </si>
   <si>
     <t>Defect ID</t>
@@ -412,6 +409,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -423,9 +423,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +704,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -725,14 +722,14 @@
     <col min="9" max="9" width="80.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -741,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>2</v>
@@ -750,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>4</v>
@@ -761,9 +758,7 @@
       <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -774,38 +769,37 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
+    </row>
+    <row r="5" spans="1:21" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>30</v>
+      <c r="I5" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -816,24 +810,23 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+    </row>
+    <row r="6" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -844,26 +837,25 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -874,26 +866,25 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -904,26 +895,25 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -934,24 +924,23 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+    </row>
+    <row r="10" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -962,36 +951,35 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:21" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1002,36 +990,35 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1042,18 +1029,17 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1061,7 +1047,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1072,18 +1058,17 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-    </row>
-    <row r="14" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1091,7 +1076,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1102,9 +1087,8 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1125,9 +1109,8 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1148,9 +1131,8 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1171,9 +1153,8 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1194,7 +1175,6 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>